<commit_message>
chore: add codesandbox example
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -55,11 +55,11 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <color rgb="d10808"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <color rgb="d10808"/>
     </font>
   </fonts>
   <fills count="3">
@@ -568,11 +568,11 @@
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="87.83203125" customWidth="1"/>
+    <col min="8" max="8" width="75.83203125" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
     <col min="11" max="11" width="20.83203125" customWidth="1"/>
@@ -622,37 +622,37 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Boris</v>
+        <v>Jewell</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>White</v>
+        <v>Schaefer</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Amos_Roob88@hotmail.com</v>
+        <v>Wilhelmine.Miller@gmail.com</v>
       </c>
       <c r="E2" s="5" t="str">
-        <v>manager</v>
+        <v>admin, manager</v>
       </c>
       <c r="F2" s="6">
-        <v>562882.73</v>
+        <v>502387.05</v>
       </c>
       <c r="G2" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4" t="str">
-        <v>Bergnaum Group, Gerlach, Corwin and Huel, Fahey Inc, Mohr - Rau</v>
+        <v/>
       </c>
       <c r="I2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4" t="str">
         <v>N/A</v>
       </c>
       <c r="L2" s="8">
-        <v>45050.949964039355</v>
+        <v>45059.20959097222</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
@@ -660,37 +660,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="str">
-        <v>Darrion</v>
+        <v>Deven</v>
       </c>
       <c r="C3" s="4" t="str">
-        <v>Ruecker</v>
+        <v>Treutel</v>
       </c>
       <c r="D3" s="4" t="str">
-        <v>Raegan97@gmail.com</v>
+        <v>Rosalinda.Feest37@yahoo.com</v>
       </c>
       <c r="E3" s="9" t="str">
-        <v>admin, user, manager, guest</v>
+        <v>guest</v>
       </c>
       <c r="F3" s="6">
-        <v>529476.04</v>
+        <v>588916.97</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="4" t="str">
-        <v>Bednar and Sons, Gislason, Wisozk and Lebsack</v>
+        <v>Macejkovic LLC, Watsica, Ankunding and Kirlin, Hills, Paucek and Feest</v>
       </c>
       <c r="I3" s="7">
         <v>8</v>
       </c>
       <c r="J3" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K3" s="4" t="str">
         <v>N/A</v>
       </c>
       <c r="L3" s="8">
-        <v>45160.81211396991</v>
+        <v>45164.5944452662</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
@@ -698,37 +698,37 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Kaitlin</v>
+        <v>Florida</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Gleichner</v>
+        <v>Durgan</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Arlene.Leffler10@hotmail.com</v>
+        <v>Annabelle.Russel@gmail.com</v>
       </c>
       <c r="E4" s="9" t="str">
-        <v>admin, manager, guest</v>
+        <v>user, manager</v>
       </c>
       <c r="F4" s="6">
-        <v>46610.6</v>
+        <v>234606.01</v>
       </c>
       <c r="G4" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4" t="str">
-        <v>Kling, Schamberger and Shanahan, Rogahn - Johnson</v>
+        <v/>
       </c>
       <c r="I4" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J4" s="4">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4" t="str">
-        <v>N/A</v>
+        <v>4</v>
+      </c>
+      <c r="K4" s="4">
+        <v>5</v>
       </c>
       <c r="L4" s="8">
-        <v>44965.59511797454</v>
+        <v>45037.156146863425</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
@@ -736,37 +736,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="str">
-        <v>Juanita</v>
+        <v>Kasey</v>
       </c>
       <c r="C5" s="4" t="str">
-        <v>Reilly</v>
+        <v>Pfeffer</v>
       </c>
       <c r="D5" s="4" t="str">
-        <v>Jamie_Franey36@gmail.com</v>
-      </c>
-      <c r="E5" s="9" t="str">
-        <v>admin, user, manager, guest</v>
+        <v>Zula2@hotmail.com</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>admin, manager</v>
       </c>
       <c r="F5" s="6">
-        <v>315261.17</v>
+        <v>223373.99</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4" t="str">
-        <v/>
+        <v>Crist - Runolfsdottir</v>
       </c>
       <c r="I5" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J5" s="4">
-        <v>9</v>
-      </c>
-      <c r="K5" s="4" t="str">
-        <v>N/A</v>
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>8</v>
       </c>
       <c r="L5" s="8">
-        <v>45224.975095497684</v>
+        <v>45154.28490810185</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
@@ -774,37 +774,37 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Raquel</v>
+        <v>Salvatore</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Maggio</v>
+        <v>Feest</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>Syble.Marquardt79@yahoo.com</v>
-      </c>
-      <c r="E6" s="5" t="str">
+        <v>Amely.Hilpert@gmail.com</v>
+      </c>
+      <c r="E6" s="9" t="str">
         <v>manager, guest</v>
       </c>
       <c r="F6" s="6">
-        <v>515586.81</v>
+        <v>582290.16</v>
       </c>
       <c r="G6" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="4" t="str">
-        <v>Rau, Rolfson and Gibson</v>
+        <v>Donnelly Inc, Miller LLC, Morar Inc</v>
       </c>
       <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
         <v>4</v>
       </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
       <c r="K6" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6" s="8">
-        <v>44934.93865380787</v>
+        <v>44922.9991275</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
@@ -812,37 +812,37 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="str">
-        <v>Monserrat</v>
+        <v>Vladimir</v>
       </c>
       <c r="C7" s="4" t="str">
-        <v>Labadie</v>
+        <v>DuBuque</v>
       </c>
       <c r="D7" s="4" t="str">
-        <v>Roman72@gmail.com</v>
+        <v>Bryon_Ankunding9@hotmail.com</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>manager, guest</v>
+        <v>admin</v>
       </c>
       <c r="F7" s="6">
-        <v>537157.28</v>
+        <v>883169.16</v>
       </c>
       <c r="G7" s="4">
         <v>2</v>
       </c>
       <c r="H7" s="4" t="str">
-        <v>Daniel, O'Kon and Ortiz, Stanton - Gibson</v>
+        <v>Boyer Group, Kuvalis LLC</v>
       </c>
       <c r="I7" s="7">
         <v>8</v>
       </c>
       <c r="J7" s="4">
-        <v>8</v>
-      </c>
-      <c r="K7" s="4" t="str">
-        <v>N/A</v>
+        <v>3</v>
+      </c>
+      <c r="K7" s="4">
+        <v>5</v>
       </c>
       <c r="L7" s="8">
-        <v>44942.71157709491</v>
+        <v>45125.20094164352</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
@@ -850,37 +850,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Willie</v>
+        <v>Toy</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Langworth</v>
+        <v>Gislason</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>Nakia.Hickle@hotmail.com</v>
+        <v>Marques_Luettgen@gmail.com</v>
       </c>
       <c r="E8" s="9" t="str">
-        <v>admin, user, guest</v>
+        <v>user, manager</v>
       </c>
       <c r="F8" s="6">
-        <v>313614</v>
+        <v>784932.57</v>
       </c>
       <c r="G8" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4" t="str">
-        <v>Collins and Sons, Blanda and Sons, Marks and Sons</v>
+        <v>Mraz LLC</v>
       </c>
       <c r="I8" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="4" t="str">
-        <v>N/A</v>
+      <c r="K8" s="4">
+        <v>0</v>
       </c>
       <c r="L8" s="8">
-        <v>45074.400084166664</v>
+        <v>45185.64358398148</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
@@ -888,37 +888,37 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="str">
-        <v>Meghan</v>
+        <v>Collin</v>
       </c>
       <c r="C9" s="4" t="str">
-        <v>Hammes</v>
+        <v>Waelchi</v>
       </c>
       <c r="D9" s="4" t="str">
-        <v>Ferne.Kihn20@yahoo.com</v>
+        <v>Anais.Bergnaum@gmail.com</v>
       </c>
       <c r="E9" s="9" t="str">
-        <v>admin, user, manager, guest</v>
+        <v>manager</v>
       </c>
       <c r="F9" s="6">
-        <v>373682.1</v>
+        <v>338715.98</v>
       </c>
       <c r="G9" s="4">
         <v>4</v>
       </c>
       <c r="H9" s="4" t="str">
-        <v>Armstrong - Mertz, Mraz Inc, Lindgren, Emard and Ryan, Kessler, Homenick and Hilll</v>
+        <v>McCullough Group, Cartwright Inc, Abernathy Group, Berge Inc</v>
       </c>
       <c r="I9" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J9" s="4">
-        <v>4</v>
-      </c>
-      <c r="K9" s="4" t="str">
-        <v>N/A</v>
+        <v>7</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3</v>
       </c>
       <c r="L9" s="8">
-        <v>44998.5254146875</v>
+        <v>45023.99084547454</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
@@ -926,37 +926,37 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Mabelle</v>
+        <v>Casimir</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Reichert</v>
+        <v>Dietrich</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>Zella_Willms-Konopelski@hotmail.com</v>
+        <v>Jazmyn.Bogisich52@hotmail.com</v>
       </c>
       <c r="E10" s="9" t="str">
-        <v>admin, user, guest</v>
+        <v>manager, guest</v>
       </c>
       <c r="F10" s="6">
-        <v>762565.15</v>
+        <v>885701.75</v>
       </c>
       <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="I10" s="7">
+        <v>6</v>
+      </c>
+      <c r="J10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="4" t="str">
-        <v>Bashirian Group</v>
-      </c>
-      <c r="I10" s="7">
+      <c r="K10" s="4">
         <v>7</v>
       </c>
-      <c r="J10" s="4">
-        <v>2</v>
-      </c>
-      <c r="K10" s="4" t="str">
-        <v>N/A</v>
-      </c>
       <c r="L10" s="8">
-        <v>45076.00578954861</v>
+        <v>44991.15771571759</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
@@ -964,37 +964,37 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="str">
-        <v>Nina</v>
+        <v>Kirsten</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>Schinner</v>
+        <v>White</v>
       </c>
       <c r="D11" s="4" t="str">
-        <v>Shayne.Nader@yahoo.com</v>
+        <v>Ruth_Mitchell25@hotmail.com</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>guest</v>
+        <v>admin</v>
       </c>
       <c r="F11" s="6">
-        <v>890979.82</v>
+        <v>937222.48</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4" t="str">
-        <v/>
+        <v>Monahan LLC</v>
       </c>
       <c r="I11" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="str">
+        <v>N/A</v>
       </c>
       <c r="L11" s="8">
-        <v>44999.13215576389</v>
+        <v>45153.52713135417</v>
       </c>
     </row>
   </sheetData>
@@ -1013,7 +1013,7 @@
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1029,112 +1029,112 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>Boris</v>
+        <v>Jewell</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>White</v>
+        <v>Schaefer</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>Amos_Roob88@hotmail.com</v>
+        <v>Wilhelmine.Miller@gmail.com</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="4" t="str">
-        <v>Darrion</v>
+        <v>Deven</v>
       </c>
       <c r="B3" s="4" t="str">
-        <v>Ruecker</v>
+        <v>Treutel</v>
       </c>
       <c r="C3" s="4" t="str">
-        <v>Raegan97@gmail.com</v>
+        <v>Rosalinda.Feest37@yahoo.com</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="4" t="str">
-        <v>Kaitlin</v>
+        <v>Florida</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Gleichner</v>
+        <v>Durgan</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Arlene.Leffler10@hotmail.com</v>
+        <v>Annabelle.Russel@gmail.com</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>Juanita</v>
+        <v>Kasey</v>
       </c>
       <c r="B5" s="4" t="str">
-        <v>Reilly</v>
+        <v>Pfeffer</v>
       </c>
       <c r="C5" s="4" t="str">
-        <v>Jamie_Franey36@gmail.com</v>
+        <v>Zula2@hotmail.com</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="4" t="str">
-        <v>Raquel</v>
+        <v>Salvatore</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Maggio</v>
+        <v>Feest</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Syble.Marquardt79@yahoo.com</v>
+        <v>Amely.Hilpert@gmail.com</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="str">
-        <v>Monserrat</v>
+        <v>Vladimir</v>
       </c>
       <c r="B7" s="4" t="str">
-        <v>Labadie</v>
+        <v>DuBuque</v>
       </c>
       <c r="C7" s="4" t="str">
-        <v>Roman72@gmail.com</v>
+        <v>Bryon_Ankunding9@hotmail.com</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>Willie</v>
+        <v>Toy</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Langworth</v>
+        <v>Gislason</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Nakia.Hickle@hotmail.com</v>
+        <v>Marques_Luettgen@gmail.com</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="4" t="str">
-        <v>Meghan</v>
+        <v>Collin</v>
       </c>
       <c r="B9" s="4" t="str">
-        <v>Hammes</v>
+        <v>Waelchi</v>
       </c>
       <c r="C9" s="4" t="str">
-        <v>Ferne.Kihn20@yahoo.com</v>
+        <v>Anais.Bergnaum@gmail.com</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="4" t="str">
-        <v>Mabelle</v>
+        <v>Casimir</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Reichert</v>
+        <v>Dietrich</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Zella_Willms-Konopelski@hotmail.com</v>
+        <v>Jazmyn.Bogisich52@hotmail.com</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>Nina</v>
+        <v>Kirsten</v>
       </c>
       <c r="B11" s="4" t="str">
-        <v>Schinner</v>
+        <v>White</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>Shayne.Nader@yahoo.com</v>
+        <v>Ruth_Mitchell25@hotmail.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>